<commit_message>
Added & updated link budget & removed unneeded =
</commit_message>
<xml_diff>
--- a/Communication (COM)/Budgets/RCL-B-COM3.xlsx
+++ b/Communication (COM)/Budgets/RCL-B-COM3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12405" activeTab="1"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
   <si>
     <t>Inputs</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>Uplink Frequency</t>
-  </si>
-  <si>
-    <t>UHF Uplink</t>
   </si>
   <si>
     <t>Station TX power</t>
@@ -358,6 +355,36 @@
   </si>
   <si>
     <t>S/C Antenna Gain</t>
+  </si>
+  <si>
+    <t>Ground station loss of 5° and spacecraft loss of 20°</t>
+  </si>
+  <si>
+    <t>Dependent on elevation angle</t>
+  </si>
+  <si>
+    <t>Distance RF signal has to propagate</t>
+  </si>
+  <si>
+    <t>This is the uptimate measure of the receiver's performance.</t>
+  </si>
+  <si>
+    <t>This is the signal level received in space in the vacinity of the spacecraft using an omnidirectional antenna.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ground Station Effective Isotropic Radiated Power </t>
+  </si>
+  <si>
+    <t>S/C Signal-to-Noise Power Density</t>
+  </si>
+  <si>
+    <t>Energy per bit to Noise Density Ratio</t>
+  </si>
+  <si>
+    <t>50 W transmit power</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -444,7 +471,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -610,14 +637,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thick">
         <color indexed="8"/>
       </left>
       <right/>
       <top/>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -635,7 +669,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -708,22 +742,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -733,9 +758,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -748,24 +770,72 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="13" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1296,12 +1366,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1522,12 +1592,12 @@
         <v>30</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>41</v>
@@ -1675,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,7 +1761,7 @@
     <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29"/>
       <c r="B1" s="30" t="s">
         <v>60</v>
@@ -1699,13 +1769,13 @@
       <c r="C1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="54"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="31"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>63</v>
       </c>
@@ -1716,30 +1786,30 @@
         <f>uuf</f>
         <v>433</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
         <v>64</v>
-      </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>65</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="55">
+      <c r="C3" s="48">
         <f>10*LOG(GSTP)</f>
         <v>16.989700043360187</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
+      <c r="D3" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="52"/>
       <c r="F3" s="31"/>
     </row>
-    <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>66</v>
+    <row r="4" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34" t="s">
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>33</v>
@@ -1748,60 +1818,64 @@
         <f>GSG</f>
         <v>15</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
       <c r="F4" s="31"/>
     </row>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="42" t="s">
+    <row r="5" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="38">
         <f>GSL</f>
         <v>3.6</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="56"/>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="31"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="B6" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="55">
+      <c r="C6" s="63">
         <f>C3+C4-C5</f>
         <v>28.389700043360186</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
+      <c r="D6" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="56"/>
       <c r="F6" s="31"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="1:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="37">
         <f>GSPL</f>
         <v>0.2</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="37"/>
+      <c r="D7" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="58"/>
       <c r="F7" s="31"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
-        <v>72</v>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>36</v>
@@ -1810,13 +1884,13 @@
         <f>loss</f>
         <v>0.2</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="37"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54"/>
       <c r="F8" s="31"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>73</v>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>36</v>
@@ -1825,13 +1899,15 @@
         <f>AIL</f>
         <v>2.1</v>
       </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="37"/>
+      <c r="D9" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="54"/>
       <c r="F9" s="31"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>74</v>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="34" t="s">
+        <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>36</v>
@@ -1840,169 +1916,186 @@
         <f>UIS</f>
         <v>0.4</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="37"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54"/>
       <c r="F10" s="31"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="45">
+      <c r="C11" s="39">
         <f>(radEarth*(((((alt+radEarth)^2)/(radEarth^2))-(COS(RADIANS((del))))^2)^(1/2)-SIN(RADIANS(del))))/1000</f>
         <v>1499.8073057120612</v>
       </c>
-      <c r="D11" s="39"/>
-      <c r="E11" s="37"/>
+      <c r="D11" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="54"/>
       <c r="F11" s="31"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="47">
+      <c r="C12" s="41">
         <f>22+20*LOG10((C11*1000)/(c_/(uuf*10^6)))</f>
         <v>148.71405484416798</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="37"/>
+      <c r="D12" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="58"/>
       <c r="F12" s="31"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="47">
+    <row r="13" spans="1:6" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="61">
         <f>C6-SUM(C7:C10,C12)</f>
         <v>-123.22435480080779</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="37"/>
+      <c r="D13" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="58"/>
       <c r="F13" s="31"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+    <row r="14" spans="1:6" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="47">
+      <c r="C14" s="61">
         <f>SCG-SCL-10*LOG(SSNT)</f>
         <v>-21.166405073382808</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="37"/>
+      <c r="D14" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="58"/>
       <c r="F14" s="31"/>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="47">
+      <c r="C15" s="41">
         <f>C13-C7-k+C14</f>
         <v>84.009240125809399</v>
       </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="37"/>
+      <c r="D15" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="54"/>
       <c r="F15" s="31"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>83</v>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="33" t="s">
+        <v>82</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="42">
         <f>10*LOG(ul)</f>
         <v>30.791812460476248</v>
       </c>
-      <c r="D16" s="39"/>
-      <c r="E16" s="37"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="54"/>
       <c r="F16" s="31"/>
     </row>
-    <row r="17" spans="1:6" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="49" t="s">
+    <row r="17" spans="1:10" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="43">
         <f>C15-C16</f>
         <v>53.217427665333148</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="37"/>
+      <c r="D17" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="58"/>
       <c r="F17" s="31"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="51">
+      <c r="C18" s="44">
         <f>0.5*ERFC(2*(C17/SQRT(2)))</f>
         <v>0</v>
       </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="39"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="53"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="35"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="D20" s="31"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J31" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
@@ -2016,13 +2109,30 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I39" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="1">
+  <mergeCells count="18">
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="lessThan">

</xml_diff>